<commit_message>
updated activities about search algorithms for IA
</commit_message>
<xml_diff>
--- a/artificial-intelligence/exercises/IA-equipes.xlsx
+++ b/artificial-intelligence/exercises/IA-equipes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e256816d4a20c6b/Emprego/Docencia/git/teaching/artificial-intelligence/exercises/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="11_F25DC773A252ABDACC104810C9DF7D8C5BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A667ABA0-3F0A-4789-8E66-B489FE5B19CE}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="11_F25DC773A252ABDACC104810C9DF7D8C5BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A703350E-5ED6-4238-ACCF-58A4A7ED9EBE}"/>
   <bookViews>
     <workbookView xWindow="30720" yWindow="-1890" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>ID Equipe</t>
   </si>
@@ -68,6 +68,12 @@
     <t>JOAO HENRIQUE</t>
   </si>
   <si>
+    <t xml:space="preserve"> ARTUR FELIPE</t>
+  </si>
+  <si>
+    <t>JOAO VICTOR LIMA</t>
+  </si>
+  <si>
     <t>Judson Rodrigues</t>
   </si>
   <si>
@@ -105,6 +111,33 @@
   </si>
   <si>
     <t>Letícia Delfino de Araujo</t>
+  </si>
+  <si>
+    <t>ANA CAROLINA MENDES FORTES</t>
+  </si>
+  <si>
+    <t>fortes.ana@discente.ufma.br</t>
+  </si>
+  <si>
+    <t>Lucas Nattan Pereira Silva</t>
+  </si>
+  <si>
+    <t>Nargylla Fernanda Cloviel Lima</t>
+  </si>
+  <si>
+    <t>José João Monteiro Costa</t>
+  </si>
+  <si>
+    <t>Ana Clara Araujo da Cruz</t>
+  </si>
+  <si>
+    <t>ana.cac@discente.ufma.br</t>
+  </si>
+  <si>
+    <t>Arthur da Silva Sá</t>
+  </si>
+  <si>
+    <t>Bruno Ferres</t>
   </si>
 </sst>
 </file>
@@ -173,7 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -184,6 +217,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -466,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -480,7 +516,7 @@
     <col min="4" max="4" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25">
+    <row r="1" spans="1:14" ht="26.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,8 +529,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.6">
+      <c r="N1" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.6">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -505,7 +544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.6">
+    <row r="3" spans="1:14" ht="15.6">
       <c r="A3" s="4"/>
       <c r="B3" s="2">
         <v>2</v>
@@ -514,7 +553,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.6">
+    <row r="4" spans="1:14" ht="15.6">
       <c r="A4" s="4"/>
       <c r="B4" s="2">
         <v>3</v>
@@ -523,7 +562,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.6">
+    <row r="5" spans="1:14" ht="15.6">
       <c r="A5" s="4"/>
       <c r="B5" s="2">
         <v>4</v>
@@ -532,7 +571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.6">
+    <row r="6" spans="1:14" ht="15.6">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -543,7 +582,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.6">
+    <row r="7" spans="1:14" ht="15.6">
       <c r="A7" s="4"/>
       <c r="B7" s="2">
         <v>2</v>
@@ -552,57 +591,63 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75">
+    <row r="8" spans="1:14" ht="15.75">
       <c r="A8" s="4"/>
-      <c r="B8" s="2">
+      <c r="B8" s="5">
         <v>3</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.6">
+    </row>
+    <row r="9" spans="1:14" ht="15.6">
       <c r="A9" s="4"/>
       <c r="B9" s="2">
         <v>4</v>
       </c>
       <c r="C9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75">
+      <c r="A10" s="4">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.6">
-      <c r="A10" s="4">
-        <v>3</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.6">
+    <row r="11" spans="1:14" ht="15.75">
       <c r="A11" s="4"/>
       <c r="B11" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.6">
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.6">
       <c r="A12" s="4"/>
       <c r="B12" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.6">
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15.75">
       <c r="A13" s="4"/>
       <c r="B13" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.6">
+    <row r="14" spans="1:14" ht="15.6">
       <c r="A14" s="4">
         <v>4</v>
       </c>
@@ -610,25 +655,25 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15.6">
       <c r="A15" s="4"/>
       <c r="B15" s="2">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.6">
       <c r="A16" s="4"/>
       <c r="B16" s="2">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.6">
@@ -637,7 +682,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75">
@@ -648,10 +693,10 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.6">
@@ -660,7 +705,7 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.6">
@@ -669,7 +714,7 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.6">
@@ -678,15 +723,21 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75">
       <c r="A22" s="4">
         <v>6</v>
       </c>
       <c r="B22" s="2">
         <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.6">
@@ -694,11 +745,17 @@
       <c r="B23" s="2">
         <v>2</v>
       </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="15.6">
       <c r="A24" s="4"/>
       <c r="B24" s="2">
         <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.6">
@@ -706,13 +763,22 @@
       <c r="B25" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.6">
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75">
       <c r="A26" s="4">
         <v>7</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6">
@@ -720,11 +786,17 @@
       <c r="B27" s="2">
         <v>2</v>
       </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="15.6">
       <c r="A28" s="4"/>
       <c r="B28" s="2">
         <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.6">
@@ -741,7 +813,7 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.6">
@@ -768,8 +840,10 @@
     <mergeCell ref="A22:A25"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1" xr:uid="{92E91BA6-5687-4064-8EDB-BA91FE933CC2}"/>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{92E91BA6-5687-4064-8EDB-BA91FE933CC2}"/>
     <hyperlink ref="D18" r:id="rId2" xr:uid="{78398891-0F67-49F7-B728-B890A1026E8B}"/>
+    <hyperlink ref="D22" r:id="rId3" xr:uid="{E023DB7F-37E9-4280-B4B3-1E2E8367707E}"/>
+    <hyperlink ref="D26" r:id="rId4" xr:uid="{82285DC9-2A46-4902-A2C1-4942AC838490}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>